<commit_message>
Code Fake UserAgent Part 1
</commit_message>
<xml_diff>
--- a/Khảo sát trang tin tuyển dụng.xlsx
+++ b/Khảo sát trang tin tuyển dụng.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trung Nguyen\OneDrive\Desktop\DevWorkSpider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB33E7B-BB7E-4ABB-885D-A04591207353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5C1388-4DF0-4DA8-83A2-0ABC7D060385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="11070" activeTab="1" xr2:uid="{01738CA1-2BAE-4404-9411-442D8BDAE98F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{01738CA1-2BAE-4404-9411-442D8BDAE98F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Thiết kế DB" sheetId="3" r:id="rId3"/>
+    <sheet name="Khảo sát" sheetId="1" r:id="rId1"/>
+    <sheet name="CSS Selector Devwork" sheetId="2" r:id="rId2"/>
+    <sheet name="ETL Dữ liệu " sheetId="4" r:id="rId3"/>
+    <sheet name="Thiết kế DB" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="149">
   <si>
     <t xml:space="preserve">Trường </t>
   </si>
@@ -471,6 +472,28 @@
   </si>
   <si>
     <t>v ( Không có cụ thể nhưng có thời gian còn lại )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETL </t>
+  </si>
+  <si>
+    <t>.strip()</t>
+  </si>
+  <si>
+    <t>Bỏ đi \n character và khoảng trắng</t>
+  </si>
+  <si>
+    <t>Nội dung</t>
+  </si>
+  <si>
+    <t>sử dụng thư viện re để lấy ra 2 số 
+vd: 10-12 triệu -&gt; ['10','12'] -&gt; Lấy ra lương trung bình -&gt; 11</t>
+  </si>
+  <si>
+    <t>- x năm
+- Trên x năm 
+- Dưới x năm 
+- Chưa có kinh nghiệm</t>
   </si>
 </sst>
 </file>
@@ -524,12 +547,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -848,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A81F992-EB71-4923-B6F3-CCDD3EB17632}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D18" sqref="B18:D18"/>
     </sheetView>
@@ -1125,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C9314B-945E-4F79-9FD7-21270EB31E69}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1493,12 +1519,148 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B810D0EB-08A8-4A32-97EB-C37E0C61C16C}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD90621B-93AA-4455-9672-35B8A66C2E9E}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:B18"/>
+      <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
code Fake User Agent
</commit_message>
<xml_diff>
--- a/Khảo sát trang tin tuyển dụng.xlsx
+++ b/Khảo sát trang tin tuyển dụng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trung Nguyen\OneDrive\Desktop\DevWorkSpider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5C1388-4DF0-4DA8-83A2-0ABC7D060385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F047B169-1948-4B82-A9D8-4E9272D2A2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{01738CA1-2BAE-4404-9411-442D8BDAE98F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{01738CA1-2BAE-4404-9411-442D8BDAE98F}"/>
   </bookViews>
   <sheets>
     <sheet name="Khảo sát" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
   <si>
     <t xml:space="preserve">Trường </t>
   </si>
@@ -494,6 +494,10 @@
 - Trên x năm 
 - Dưới x năm 
 - Chưa có kinh nghiệm</t>
+  </si>
+  <si>
+    <t>+Cách 1: sử dụng thư viện re , dùng re.findall()
++Cách 2 : Sử lý chuỗi dùng split(), replace()</t>
   </si>
 </sst>
 </file>
@@ -547,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -556,6 +560,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1522,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B810D0EB-08A8-4A32-97EB-C37E0C61C16C}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1622,6 +1629,9 @@
       </c>
       <c r="B14" s="5" t="s">
         <v>148</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ETL Data part 1
</commit_message>
<xml_diff>
--- a/Khảo sát trang tin tuyển dụng.xlsx
+++ b/Khảo sát trang tin tuyển dụng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trung Nguyen\OneDrive\Desktop\DevWorkSpider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F047B169-1948-4B82-A9D8-4E9272D2A2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00860F30-C6A2-48BE-A694-ADF02671E4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{01738CA1-2BAE-4404-9411-442D8BDAE98F}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="151">
   <si>
     <t xml:space="preserve">Trường </t>
   </si>
@@ -498,6 +498,11 @@
   <si>
     <t>+Cách 1: sử dụng thư viện re , dùng re.findall()
 +Cách 2 : Sử lý chuỗi dùng split(), replace()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ x-x triệu 
++ Dưới x triệu 
++ Trên x triệu </t>
   </si>
 </sst>
 </file>
@@ -1530,7 +1535,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1618,7 +1623,9 @@
       <c r="A13" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>147</v>
       </c>

</xml_diff>